<commit_message>
machine learning listo, no tocar
</commit_message>
<xml_diff>
--- a/backend/datos_modelo.xlsx
+++ b/backend/datos_modelo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaco\OneDrive\Escritorio\RAMOS\CAPSTONE\Aplicacion\diagnostico_de_cancer\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaco\OneDrive\Escritorio\RAMOS\CAPSTONE\Aplicacion\diagnostico_de_cancer_ml\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91B03904-FBEF-4E95-91C6-6412B6D0FF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D64965-A4D2-4D8B-9F68-56287205A1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="3840" windowWidth="28800" windowHeight="15225" xr2:uid="{A11C7C91-8C99-4D16-89C4-FCF02E96A04B}"/>
+    <workbookView xWindow="3405" yWindow="7695" windowWidth="28800" windowHeight="15225" xr2:uid="{A11C7C91-8C99-4D16-89C4-FCF02E96A04B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="4" r:id="rId1"/>
@@ -936,9 +936,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1256,7 +1255,7 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I61"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,10 +1337,10 @@
       <c r="G2" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2">
         <v>955667788</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2">
         <v>34</v>
       </c>
       <c r="J2" t="s">
@@ -1388,10 +1387,10 @@
       <c r="G3" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3">
         <v>912233445</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3">
         <v>43</v>
       </c>
       <c r="J3" t="s">
@@ -1438,10 +1437,10 @@
       <c r="G4" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4">
         <v>345678901</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4">
         <v>33</v>
       </c>
       <c r="J4" t="s">
@@ -1488,10 +1487,10 @@
       <c r="G5" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5">
         <v>994567121</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5">
         <v>22</v>
       </c>
       <c r="J5" t="s">
@@ -1538,10 +1537,10 @@
       <c r="G6" t="s">
         <v>84</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6">
         <v>1122334</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6">
         <v>25</v>
       </c>
       <c r="J6" t="s">
@@ -1588,10 +1587,10 @@
       <c r="G7" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7">
         <v>890123456</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7">
         <v>43</v>
       </c>
       <c r="J7" t="s">
@@ -1638,10 +1637,10 @@
       <c r="G8" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8">
         <v>922344556</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8">
         <v>48</v>
       </c>
       <c r="J8" t="s">
@@ -1688,10 +1687,10 @@
       <c r="G9" t="s">
         <v>108</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9">
         <v>977889900</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9">
         <v>27</v>
       </c>
       <c r="J9" t="s">
@@ -1738,10 +1737,10 @@
       <c r="G10" t="s">
         <v>111</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10">
         <v>955667788</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10">
         <v>34</v>
       </c>
       <c r="J10" t="s">
@@ -1788,10 +1787,10 @@
       <c r="G11" t="s">
         <v>115</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11">
         <v>944556677</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11">
         <v>29</v>
       </c>
       <c r="J11" t="s">
@@ -1838,10 +1837,10 @@
       <c r="G12" t="s">
         <v>120</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12">
         <v>912233445</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12">
         <v>43</v>
       </c>
       <c r="J12" t="s">
@@ -1888,10 +1887,10 @@
       <c r="G13" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13">
         <v>994321574</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13">
         <v>34</v>
       </c>
       <c r="J13" t="s">
@@ -1938,10 +1937,10 @@
       <c r="G14" t="s">
         <v>125</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14">
         <v>944556677</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14">
         <v>29</v>
       </c>
       <c r="J14" t="s">
@@ -1988,10 +1987,10 @@
       <c r="G15" t="s">
         <v>128</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15">
         <v>955667788</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15">
         <v>34</v>
       </c>
       <c r="J15" t="s">
@@ -2038,10 +2037,10 @@
       <c r="G16" t="s">
         <v>132</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16">
         <v>991231457</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16">
         <v>34</v>
       </c>
       <c r="J16" t="s">
@@ -2088,10 +2087,10 @@
       <c r="G17" t="s">
         <v>136</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17">
         <v>998076543</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17">
         <v>41</v>
       </c>
       <c r="J17" t="s">
@@ -2138,10 +2137,10 @@
       <c r="G18" t="s">
         <v>140</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18">
         <v>987654321</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18">
         <v>48</v>
       </c>
       <c r="J18" t="s">
@@ -2188,10 +2187,10 @@
       <c r="G19" t="s">
         <v>145</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19">
         <v>991232568</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19">
         <v>38</v>
       </c>
       <c r="J19" t="s">
@@ -2238,10 +2237,10 @@
       <c r="G20" t="s">
         <v>151</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20">
         <v>654321098</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20">
         <v>28</v>
       </c>
       <c r="J20" t="s">
@@ -2288,10 +2287,10 @@
       <c r="G21" t="s">
         <v>155</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21">
         <v>944556677</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21">
         <v>29</v>
       </c>
       <c r="J21" t="s">
@@ -2338,10 +2337,10 @@
       <c r="G22" t="s">
         <v>159</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22">
         <v>991256783</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22">
         <v>31</v>
       </c>
       <c r="J22" t="s">
@@ -2388,10 +2387,10 @@
       <c r="G23" t="s">
         <v>162</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23">
         <v>990312456</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23">
         <v>27</v>
       </c>
       <c r="J23" t="s">
@@ -2438,10 +2437,10 @@
       <c r="G24" t="s">
         <v>164</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24">
         <v>922344556</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24">
         <v>48</v>
       </c>
       <c r="J24" t="s">
@@ -2488,10 +2487,10 @@
       <c r="G25" t="s">
         <v>166</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25">
         <v>990011223</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25">
         <v>41</v>
       </c>
       <c r="J25" t="s">
@@ -2538,10 +2537,10 @@
       <c r="G26" t="s">
         <v>169</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26">
         <v>991324567</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26">
         <v>25</v>
       </c>
       <c r="J26" t="s">
@@ -2588,10 +2587,10 @@
       <c r="G27" t="s">
         <v>174</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27">
         <v>997809675</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27">
         <v>42</v>
       </c>
       <c r="J27" t="s">
@@ -2638,10 +2637,10 @@
       <c r="G28" t="s">
         <v>177</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28">
         <v>988990011</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28">
         <v>38</v>
       </c>
       <c r="J28" t="s">
@@ -2688,10 +2687,10 @@
       <c r="G29" t="s">
         <v>182</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29">
         <v>789012345</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29">
         <v>49</v>
       </c>
       <c r="J29" t="s">
@@ -2738,10 +2737,10 @@
       <c r="G30" t="s">
         <v>188</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30">
         <v>998067423</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30">
         <v>23</v>
       </c>
       <c r="J30" t="s">
@@ -2788,10 +2787,10 @@
       <c r="G31" t="s">
         <v>194</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31">
         <v>933445667</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I31">
         <v>23</v>
       </c>
       <c r="J31" t="s">
@@ -2838,10 +2837,10 @@
       <c r="G32" t="s">
         <v>196</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32">
         <v>933445667</v>
       </c>
-      <c r="I32" s="1">
+      <c r="I32">
         <v>23</v>
       </c>
       <c r="J32" t="s">
@@ -2888,10 +2887,10 @@
       <c r="G33" t="s">
         <v>199</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H33">
         <v>912341234</v>
       </c>
-      <c r="I33" s="1">
+      <c r="I33">
         <v>37</v>
       </c>
       <c r="J33" t="s">
@@ -2938,10 +2937,10 @@
       <c r="G34" t="s">
         <v>202</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H34">
         <v>988990112</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I34">
         <v>38</v>
       </c>
       <c r="J34" t="s">
@@ -2988,10 +2987,10 @@
       <c r="G35" t="s">
         <v>205</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H35">
         <v>112233344</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I35">
         <v>25</v>
       </c>
       <c r="J35" t="s">
@@ -3038,10 +3037,10 @@
       <c r="G36" t="s">
         <v>208</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H36">
         <v>922344556</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I36">
         <v>48</v>
       </c>
       <c r="J36" t="s">
@@ -3088,10 +3087,10 @@
       <c r="G37" t="s">
         <v>212</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37">
         <v>990808959</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I37">
         <v>41</v>
       </c>
       <c r="J37" t="s">
@@ -3138,10 +3137,10 @@
       <c r="G38" t="s">
         <v>215</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H38">
         <v>990856789</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I38">
         <v>28</v>
       </c>
       <c r="J38" t="s">
@@ -3188,10 +3187,10 @@
       <c r="G39" t="s">
         <v>219</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39">
         <v>990567832</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I39">
         <v>31</v>
       </c>
       <c r="J39" t="s">
@@ -3238,10 +3237,10 @@
       <c r="G40" t="s">
         <v>223</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H40">
         <v>966778990</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I40">
         <v>42</v>
       </c>
       <c r="J40" t="s">
@@ -3288,10 +3287,10 @@
       <c r="G41" t="s">
         <v>226</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H41">
         <v>990789069</v>
       </c>
-      <c r="I41" s="1">
+      <c r="I41">
         <v>25</v>
       </c>
       <c r="J41" t="s">
@@ -3338,10 +3337,10 @@
       <c r="G42" t="s">
         <v>230</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H42">
         <v>994525678</v>
       </c>
-      <c r="I42" s="1">
+      <c r="I42">
         <v>36</v>
       </c>
       <c r="J42" t="s">
@@ -3388,10 +3387,10 @@
       <c r="G43" t="s">
         <v>234</v>
       </c>
-      <c r="H43" s="1">
+      <c r="H43">
         <v>567890123</v>
       </c>
-      <c r="I43" s="1">
+      <c r="I43">
         <v>29</v>
       </c>
       <c r="J43" t="s">
@@ -3438,10 +3437,10 @@
       <c r="G44" t="s">
         <v>237</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H44">
         <v>456789012</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I44">
         <v>32</v>
       </c>
       <c r="J44" t="s">
@@ -3488,10 +3487,10 @@
       <c r="G45" t="s">
         <v>241</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H45">
         <v>990545608</v>
       </c>
-      <c r="I45" s="1">
+      <c r="I45">
         <v>42</v>
       </c>
       <c r="J45" t="s">
@@ -3538,10 +3537,10 @@
       <c r="G46" t="s">
         <v>19</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H46">
         <v>990563511</v>
       </c>
-      <c r="I46" s="1">
+      <c r="I46">
         <v>41</v>
       </c>
       <c r="J46" t="s">
@@ -3588,10 +3587,10 @@
       <c r="G47" t="s">
         <v>245</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H47">
         <v>990897549</v>
       </c>
-      <c r="I47" s="1">
+      <c r="I47">
         <v>30</v>
       </c>
       <c r="J47" t="s">
@@ -3638,10 +3637,10 @@
       <c r="G48" t="s">
         <v>248</v>
       </c>
-      <c r="H48" s="1">
+      <c r="H48">
         <v>993214569</v>
       </c>
-      <c r="I48" s="1">
+      <c r="I48">
         <v>39</v>
       </c>
       <c r="J48" t="s">
@@ -3688,10 +3687,10 @@
       <c r="G49" t="s">
         <v>18</v>
       </c>
-      <c r="H49" s="1">
+      <c r="H49">
         <v>997098799</v>
       </c>
-      <c r="I49" s="1">
+      <c r="I49">
         <v>27</v>
       </c>
       <c r="J49" t="s">
@@ -3738,10 +3737,10 @@
       <c r="G50" t="s">
         <v>253</v>
       </c>
-      <c r="H50" s="1">
+      <c r="H50">
         <v>977889900</v>
       </c>
-      <c r="I50" s="1">
+      <c r="I50">
         <v>27</v>
       </c>
       <c r="J50" t="s">
@@ -3788,10 +3787,10 @@
       <c r="G51" t="s">
         <v>256</v>
       </c>
-      <c r="H51" s="1">
+      <c r="H51">
         <v>912345678</v>
       </c>
-      <c r="I51" s="1">
+      <c r="I51">
         <v>43</v>
       </c>
       <c r="J51" t="s">
@@ -3838,10 +3837,10 @@
       <c r="G52" t="s">
         <v>260</v>
       </c>
-      <c r="H52" s="1">
+      <c r="H52">
         <v>123456789</v>
       </c>
-      <c r="I52" s="1">
+      <c r="I52">
         <v>56</v>
       </c>
       <c r="J52" t="s">
@@ -3888,10 +3887,10 @@
       <c r="G53" t="s">
         <v>23</v>
       </c>
-      <c r="H53" s="1">
+      <c r="H53">
         <v>678943579</v>
       </c>
-      <c r="I53" s="1">
+      <c r="I53">
         <v>26</v>
       </c>
       <c r="J53" t="s">
@@ -3938,10 +3937,10 @@
       <c r="G54" t="s">
         <v>268</v>
       </c>
-      <c r="H54" s="1">
+      <c r="H54">
         <v>998123126</v>
       </c>
-      <c r="I54" s="1">
+      <c r="I54">
         <v>38</v>
       </c>
       <c r="J54" t="s">
@@ -3988,10 +3987,10 @@
       <c r="G55" t="s">
         <v>271</v>
       </c>
-      <c r="H55" s="1">
+      <c r="H55">
         <v>933445667</v>
       </c>
-      <c r="I55" s="1">
+      <c r="I55">
         <v>23</v>
       </c>
       <c r="J55" t="s">
@@ -4038,10 +4037,10 @@
       <c r="G56" t="s">
         <v>274</v>
       </c>
-      <c r="H56" s="1">
+      <c r="H56">
         <v>912233445</v>
       </c>
-      <c r="I56" s="1">
+      <c r="I56">
         <v>43</v>
       </c>
       <c r="J56" t="s">
@@ -4088,10 +4087,10 @@
       <c r="G57" t="s">
         <v>277</v>
       </c>
-      <c r="H57" s="1">
+      <c r="H57">
         <v>990112233</v>
       </c>
-      <c r="I57" s="1">
+      <c r="I57">
         <v>41</v>
       </c>
       <c r="J57" t="s">
@@ -4138,10 +4137,10 @@
       <c r="G58" t="s">
         <v>279</v>
       </c>
-      <c r="H58" s="1">
+      <c r="H58">
         <v>966778899</v>
       </c>
-      <c r="I58" s="1">
+      <c r="I58">
         <v>42</v>
       </c>
       <c r="J58" t="s">
@@ -4188,10 +4187,10 @@
       <c r="G59" t="s">
         <v>282</v>
       </c>
-      <c r="H59" s="1">
+      <c r="H59">
         <v>998321456</v>
       </c>
-      <c r="I59" s="1">
+      <c r="I59">
         <v>25</v>
       </c>
       <c r="J59" t="s">
@@ -4238,10 +4237,10 @@
       <c r="G60" t="s">
         <v>285</v>
       </c>
-      <c r="H60" s="1">
+      <c r="H60">
         <v>234567890</v>
       </c>
-      <c r="I60" s="1">
+      <c r="I60">
         <v>37</v>
       </c>
       <c r="J60" t="s">
@@ -4288,10 +4287,10 @@
       <c r="G61" t="s">
         <v>288</v>
       </c>
-      <c r="H61" s="1">
+      <c r="H61">
         <v>997806995</v>
       </c>
-      <c r="I61" s="1">
+      <c r="I61">
         <v>29</v>
       </c>
       <c r="J61" t="s">

</xml_diff>